<commit_message>
added code for getting species lists from worms
</commit_message>
<xml_diff>
--- a/data/Artsprioritering_v05_2024sep.xlsx
+++ b/data/Artsprioritering_v05_2024sep.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1048" uniqueCount="210">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1048" uniqueCount="225">
   <si>
     <t xml:space="preserve">Table 1. Prioritized list of NIS to target</t>
   </si>
@@ -612,18 +612,33 @@
     <t xml:space="preserve">PrNr</t>
   </si>
   <si>
+    <t xml:space="preserve">Crassostrea virginica (Gmelin, 1791)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mytilopsis leucophaeata (Conrad, 1831)</t>
+  </si>
+  <si>
     <t xml:space="preserve">Clusa et al., 2017</t>
   </si>
   <si>
     <t xml:space="preserve">Clusa L, Miralles L, Basanta A, Escot C, García-Vázquez E (2017) eDNA for detection of five highly invasive molluscs. A case study in urban rivers from the Iberian Peninsula. PLOS ONE 12(11): e0188126. https://doi.org/10.1371/journal.pone.0188126</t>
   </si>
   <si>
+    <t xml:space="preserve">Acipenser ruthenus Linnaeus, 1758</t>
+  </si>
+  <si>
     <t xml:space="preserve">Schenekar et al., 2020</t>
   </si>
   <si>
     <t xml:space="preserve">Schenekar, T., Schletterer, M. &amp; Weiss, S.J. Development of a TaqMan qPCR protocol for detecting Acipenser ruthenus in the Volga headwaters from eDNA samples. Conservation Genet Resour 12, 395–397 (2020). https://doi.org/10.1007/s12686-020-01128-w</t>
   </si>
   <si>
+    <t xml:space="preserve">Acipenser transmontanus Richardson, 1836</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Potamopyrgus antipodarum (Gray, 1843)</t>
+  </si>
+  <si>
     <t xml:space="preserve">Goldberg et al.,  2013</t>
   </si>
   <si>
@@ -636,22 +651,52 @@
     <t xml:space="preserve">Miralles, L., Parrondo, M., Hernández de Rojas, A., Garcia-Vazquez, E., &amp; Borrell, Y. J. (2019). Development and validation of eDNA markers for the detection of Crepidula fornicata in environmental samples. Marine pollution bulletin, 146, 827–830. https://doi.org/10.1016/j.marpolbul.2019.07.050</t>
   </si>
   <si>
+    <t xml:space="preserve">Heterosigma akashiwo (Y.Hada) Y.Hada ex Y.Hara &amp; M.Chihara, 1987</t>
+  </si>
+  <si>
     <t xml:space="preserve">Engesmo et al., 2018</t>
   </si>
   <si>
     <t xml:space="preserve">Engesmo, A., Strand, D., Gran-Stadniczeñko, S., Edvardsen, B., Medlin, L. K., &amp; Eikrem, W. (2018). Development of a qPCR assay to detect and quantify ichthyotoxic flagellates along the Norwegian coast, and the first Norwegian record of Fibrocapsa japonica (Raphidophyceae). Harmful algae, 75, 105–117. https://doi.org/10.1016/j.hal.2018.04.007</t>
   </si>
   <si>
+    <t xml:space="preserve">Fibrocapsa japonica S.Toriumi &amp; H.Takano, 1973</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dasya baillouviana (S.G.Gmelin) Montagne, 1841</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dasysiphonia japonica (Yendo) H.-S.Kim, 2012</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mulinia lateralis (Say, 1822)</t>
+  </si>
+  <si>
     <t xml:space="preserve">Muha et al., 2019</t>
   </si>
   <si>
     <t xml:space="preserve">Muha, T. P., Skukan, R., Borrell, Y. J., Rico, J. M., Garcia de Leaniz, C., Garcia-Vazquez, E., &amp; Consuegra, S. (2019). Contrasting seasonal and spatial distribution of native and invasive Codium seaweed revealed by targeting species-specific eDNA. Ecology and evolution, 9(15), 8567–8579. https://doi.org/10.1002/ece3.5379</t>
   </si>
   <si>
+    <t xml:space="preserve">Fucus distichus subsp. evanescens (C.Agardh) H.T.Powell, 1957</t>
+  </si>
+  <si>
     <t xml:space="preserve">Vandersea et al., 2017</t>
   </si>
   <si>
     <t xml:space="preserve">Vandersea, M. W., Kibler, S. R., Van Sant, S. B., Tester, P. A., Sullivan, K., Eckert, G., Cammarata, C., Reece, K., Scott, G., Place, A., Holderied, K., Hondolero, D., &amp; Litaker, R. W. (2017). qPCR assays for Alexandrium fundyense and A. ostenfeldii (Dinophyceae) identified from Alaskan waters and a review of species-specific Alexandrium molecular assays. Phycologia, 56(3), 303–320. https://doi.org/10.2216/16-41.1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Prorocentrum triestinum J.Schiller, 1918</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Echinogammarus trichiatus (Martynov, 1932)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Obesogammarus crassus (G.O. Sars, 1894)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Akashiwo sanguinea (K.Hirasaka) Gert Hansen &amp; Moestrup, 2000</t>
   </si>
 </sst>
 </file>
@@ -882,15 +927,6 @@
     <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
     <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
-  <dxfs count="1">
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="00FFFFFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-  </dxfs>
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
@@ -962,10 +998,10 @@
   <dimension ref="A2:AMJ52"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="Q30" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B7" activeCellId="1" sqref="A3 B7"/>
+      <selection pane="topLeft" activeCell="B7" activeCellId="10" sqref="E6 E9 E11:E12 E14 E18:E19 E23:E24 E26 E28 E36 E41:E42 B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.7421875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.7578125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="64.88"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="3" style="0" width="4.9"/>
@@ -4262,8 +4298,8 @@
   </sheetPr>
   <dimension ref="A3:W52"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C35" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A5" activeCellId="1" sqref="A3 A5"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C6" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E11" activeCellId="2" sqref="E6 E9 E11:E12 E14 E18:E19 E23:E24 E26 E28 E36 E41:E42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="19.7" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4415,7 +4451,7 @@
         <v>29</v>
       </c>
       <c r="E6" s="22" t="s">
-        <v>27</v>
+        <v>196</v>
       </c>
       <c r="F6" s="23" t="s">
         <v>28</v>
@@ -4607,7 +4643,7 @@
         <v>47</v>
       </c>
       <c r="E9" s="22" t="s">
-        <v>45</v>
+        <v>197</v>
       </c>
       <c r="F9" s="23" t="s">
         <v>46</v>
@@ -4655,10 +4691,10 @@
         <v>3</v>
       </c>
       <c r="U9" s="23" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="V9" s="23" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
       <c r="W9" s="19" t="s">
         <v>49</v>
@@ -4742,7 +4778,7 @@
         <v>57</v>
       </c>
       <c r="E11" s="22" t="s">
-        <v>56</v>
+        <v>200</v>
       </c>
       <c r="F11" s="23" t="s">
         <v>46</v>
@@ -4787,10 +4823,10 @@
         <v>9</v>
       </c>
       <c r="U11" s="23" t="s">
-        <v>198</v>
+        <v>201</v>
       </c>
       <c r="V11" s="23" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="W11" s="19" t="s">
         <v>59</v>
@@ -4810,7 +4846,7 @@
         <v>57</v>
       </c>
       <c r="E12" s="22" t="s">
-        <v>60</v>
+        <v>203</v>
       </c>
       <c r="F12" s="23" t="s">
         <v>46</v>
@@ -4938,7 +4974,7 @@
         <v>64</v>
       </c>
       <c r="E14" s="22" t="s">
-        <v>62</v>
+        <v>204</v>
       </c>
       <c r="F14" s="23" t="s">
         <v>28</v>
@@ -4986,10 +5022,10 @@
         <v>9</v>
       </c>
       <c r="U14" s="23" t="s">
-        <v>200</v>
+        <v>205</v>
       </c>
       <c r="V14" s="23" t="s">
-        <v>201</v>
+        <v>206</v>
       </c>
       <c r="W14" s="19" t="s">
         <v>67</v>
@@ -5121,10 +5157,10 @@
         <v>9</v>
       </c>
       <c r="U16" s="23" t="s">
-        <v>202</v>
+        <v>207</v>
       </c>
       <c r="V16" s="23" t="s">
-        <v>203</v>
+        <v>208</v>
       </c>
       <c r="W16" s="19" t="s">
         <v>77</v>
@@ -5208,7 +5244,7 @@
         <v>84</v>
       </c>
       <c r="E18" s="22" t="s">
-        <v>83</v>
+        <v>209</v>
       </c>
       <c r="F18" s="23" t="s">
         <v>28</v>
@@ -5256,10 +5292,10 @@
         <v>15</v>
       </c>
       <c r="U18" s="23" t="s">
-        <v>204</v>
+        <v>210</v>
       </c>
       <c r="V18" s="23" t="s">
-        <v>205</v>
+        <v>211</v>
       </c>
       <c r="W18" s="19" t="s">
         <v>87</v>
@@ -5279,7 +5315,7 @@
         <v>84</v>
       </c>
       <c r="E19" s="22" t="s">
-        <v>88</v>
+        <v>212</v>
       </c>
       <c r="F19" s="23" t="s">
         <v>46</v>
@@ -5327,10 +5363,10 @@
         <v>15</v>
       </c>
       <c r="U19" s="23" t="s">
-        <v>204</v>
+        <v>210</v>
       </c>
       <c r="V19" s="23" t="s">
-        <v>205</v>
+        <v>211</v>
       </c>
       <c r="W19" s="23" t="s">
         <v>87</v>
@@ -5542,7 +5578,7 @@
         <v>102</v>
       </c>
       <c r="E23" s="22" t="s">
-        <v>101</v>
+        <v>213</v>
       </c>
       <c r="F23" s="23" t="s">
         <v>28</v>
@@ -5606,7 +5642,7 @@
         <v>102</v>
       </c>
       <c r="E24" s="22" t="s">
-        <v>106</v>
+        <v>214</v>
       </c>
       <c r="F24" s="23" t="s">
         <v>28</v>
@@ -5713,7 +5749,7 @@
         <v>111</v>
       </c>
       <c r="E26" s="22" t="s">
-        <v>110</v>
+        <v>215</v>
       </c>
       <c r="F26" s="23" t="s">
         <v>46</v>
@@ -5825,10 +5861,10 @@
         <v>43</v>
       </c>
       <c r="U27" s="23" t="s">
-        <v>206</v>
+        <v>216</v>
       </c>
       <c r="V27" s="23" t="s">
-        <v>207</v>
+        <v>217</v>
       </c>
       <c r="W27" s="19" t="s">
         <v>117</v>
@@ -5848,7 +5884,7 @@
         <v>119</v>
       </c>
       <c r="E28" s="22" t="s">
-        <v>118</v>
+        <v>218</v>
       </c>
       <c r="F28" s="23" t="s">
         <v>28</v>
@@ -6149,10 +6185,10 @@
         <v>56</v>
       </c>
       <c r="U32" s="23" t="s">
-        <v>208</v>
+        <v>219</v>
       </c>
       <c r="V32" s="23" t="s">
-        <v>209</v>
+        <v>220</v>
       </c>
       <c r="W32" s="19" t="s">
         <v>131</v>
@@ -6364,7 +6400,7 @@
         <v>137</v>
       </c>
       <c r="E36" s="22" t="s">
-        <v>136</v>
+        <v>221</v>
       </c>
       <c r="F36" s="23" t="s">
         <v>28</v>
@@ -6684,7 +6720,7 @@
         <v>154</v>
       </c>
       <c r="E41" s="22" t="s">
-        <v>153</v>
+        <v>222</v>
       </c>
       <c r="F41" s="23" t="s">
         <v>46</v>
@@ -6748,7 +6784,7 @@
         <v>156</v>
       </c>
       <c r="E42" s="22" t="s">
-        <v>155</v>
+        <v>223</v>
       </c>
       <c r="F42" s="23" t="s">
         <v>46</v>
@@ -7175,7 +7211,7 @@
         <v>173</v>
       </c>
       <c r="E49" s="22" t="s">
-        <v>172</v>
+        <v>224</v>
       </c>
       <c r="F49" s="23" t="s">
         <v>28</v>
@@ -7317,13 +7353,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:L47"/>
+  <dimension ref="A1:L61"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A3" activeCellId="10" sqref="E6 E9 E11:E12 E14 E18:E19 E23:E24 E26 E28 E36 E41:E42 A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="26.74"/>
   </cols>
@@ -7703,7 +7739,7 @@
         <v>13</v>
       </c>
       <c r="L11" s="23" t="s">
-        <v>206</v>
+        <v>216</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -7739,7 +7775,7 @@
         <v>2</v>
       </c>
       <c r="L12" s="23" t="s">
-        <v>198</v>
+        <v>201</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -7993,7 +8029,7 @@
         <v>1</v>
       </c>
       <c r="L19" s="23" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -8139,7 +8175,7 @@
         <v>1</v>
       </c>
       <c r="L23" s="23" t="s">
-        <v>202</v>
+        <v>207</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -8177,7 +8213,7 @@
         <v>1</v>
       </c>
       <c r="L24" s="23" t="s">
-        <v>200</v>
+        <v>205</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -8393,7 +8429,7 @@
         <v>2</v>
       </c>
       <c r="L30" s="23" t="s">
-        <v>208</v>
+        <v>219</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="13.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -8827,7 +8863,7 @@
         <v>1</v>
       </c>
       <c r="L42" s="23" t="s">
-        <v>204</v>
+        <v>210</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="13.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -8865,7 +8901,7 @@
         <v>1</v>
       </c>
       <c r="L43" s="23" t="s">
-        <v>204</v>
+        <v>210</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="13.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
added worms_safe and flextable
</commit_message>
<xml_diff>
--- a/data/Artsprioritering_v05_2024sep.xlsx
+++ b/data/Artsprioritering_v05_2024sep.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1048" uniqueCount="225">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1062" uniqueCount="233">
   <si>
     <t xml:space="preserve">Table 1. Prioritized list of NIS to target</t>
   </si>
@@ -697,6 +697,30 @@
   </si>
   <si>
     <t xml:space="preserve">Akashiwo sanguinea (K.Hirasaka) Gert Hansen &amp; Moestrup, 2000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Haptophyta</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Coccolithophyceae</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Prymnesiales</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Prymnesiaceae</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Prymnesium parvum N.Carter, 1937</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Eckford-Soper &amp; Daugbjerg, 2015</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Chattonella subsalsa B.Biecheler, 1936</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Park et al., 2012</t>
   </si>
 </sst>
 </file>
@@ -706,7 +730,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="9">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -751,6 +775,13 @@
       <b val="true"/>
       <sz val="10"/>
       <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <i val="true"/>
+      <sz val="12"/>
+      <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
     </font>
@@ -821,7 +852,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="25">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -918,6 +949,10 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -997,11 +1032,11 @@
   </sheetPr>
   <dimension ref="A2:AMJ52"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="Q30" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B7" activeCellId="10" sqref="E6 E9 E11:E12 E14 E18:E19 E23:E24 E26 E28 E36 E41:E42 B7"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B8" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="P20" activeCellId="0" sqref="P20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.7578125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.77734375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="64.88"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="3" style="0" width="4.9"/>
@@ -4298,8 +4333,8 @@
   </sheetPr>
   <dimension ref="A3:W52"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C6" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E11" activeCellId="2" sqref="E6 E9 E11:E12 E14 E18:E19 E23:E24 E26 E28 E36 E41:E42"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F33" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="U51" activeCellId="0" sqref="U51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="19.7" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -7261,82 +7296,101 @@
       <c r="U49" s="23"/>
       <c r="V49" s="23"/>
     </row>
+    <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A50" s="19" t="s">
+        <v>225</v>
+      </c>
+      <c r="B50" s="19" t="s">
+        <v>226</v>
+      </c>
+      <c r="C50" s="19" t="s">
+        <v>227</v>
+      </c>
+      <c r="D50" s="19" t="s">
+        <v>228</v>
+      </c>
+      <c r="E50" s="19" t="s">
+        <v>229</v>
+      </c>
+      <c r="F50" s="19" t="s">
+        <v>28</v>
+      </c>
+      <c r="G50" s="19" t="n">
+        <v>1</v>
+      </c>
+      <c r="H50" s="19" t="n">
+        <v>1</v>
+      </c>
+      <c r="I50" s="19" t="n">
+        <v>1</v>
+      </c>
+      <c r="J50" s="19" t="n">
+        <v>1</v>
+      </c>
+      <c r="K50" s="19" t="n">
+        <v>1</v>
+      </c>
+      <c r="L50" s="19" t="n">
+        <v>1</v>
+      </c>
+      <c r="M50" s="19" t="n">
+        <v>1</v>
+      </c>
+      <c r="N50" s="19" t="n">
+        <v>1</v>
+      </c>
+      <c r="U50" s="19" t="s">
+        <v>230</v>
+      </c>
+    </row>
     <row r="51" customFormat="false" ht="19.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F51" s="19" t="n">
-        <f aca="false">MIN(F$6:F$49)</f>
-        <v>0</v>
+      <c r="A51" s="19" t="s">
+        <v>74</v>
+      </c>
+      <c r="B51" s="19" t="s">
+        <v>86</v>
+      </c>
+      <c r="C51" s="19" t="s">
+        <v>85</v>
+      </c>
+      <c r="D51" s="19" t="s">
+        <v>84</v>
+      </c>
+      <c r="E51" s="24" t="s">
+        <v>231</v>
+      </c>
+      <c r="F51" s="19" t="s">
+        <v>28</v>
       </c>
       <c r="G51" s="19" t="n">
-        <f aca="false">MIN(G$6:G$49)</f>
         <v>1</v>
       </c>
       <c r="H51" s="19" t="n">
-        <f aca="false">MIN(H$6:H$49)</f>
         <v>1</v>
       </c>
       <c r="I51" s="19" t="n">
-        <f aca="false">MIN(I$6:I$49)</f>
         <v>1</v>
       </c>
       <c r="J51" s="19" t="n">
-        <f aca="false">MIN(J$6:J$49)</f>
         <v>1</v>
       </c>
       <c r="K51" s="19" t="n">
-        <f aca="false">MIN(K$6:K$49)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L51" s="19" t="n">
-        <f aca="false">MIN(L$6:L$49)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M51" s="19" t="n">
-        <f aca="false">MIN(M$6:M$49)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="N51" s="19" t="n">
-        <f aca="false">MIN(N$6:N$49)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="52" customFormat="false" ht="19.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F52" s="19" t="n">
-        <f aca="false">MAX(F$6:F$49)</f>
-        <v>0</v>
-      </c>
-      <c r="G52" s="19" t="n">
-        <f aca="false">MAX(G$6:G$49)</f>
-        <v>3</v>
-      </c>
-      <c r="H52" s="19" t="n">
-        <f aca="false">MAX(H$6:H$49)</f>
-        <v>3</v>
-      </c>
-      <c r="I52" s="19" t="n">
-        <f aca="false">MAX(I$6:I$49)</f>
-        <v>3</v>
-      </c>
-      <c r="J52" s="19" t="n">
-        <f aca="false">MAX(J$6:J$49)</f>
-        <v>3</v>
-      </c>
-      <c r="K52" s="19" t="n">
-        <f aca="false">MAX(K$6:K$49)</f>
-        <v>3</v>
-      </c>
-      <c r="L52" s="19" t="n">
-        <f aca="false">MAX(L$6:L$49)</f>
-        <v>3</v>
-      </c>
-      <c r="M52" s="19" t="n">
-        <f aca="false">MAX(M$6:M$49)</f>
-        <v>6</v>
-      </c>
-      <c r="N52" s="19" t="n">
-        <f aca="false">MAX(N$6:N$49)</f>
-        <v>12</v>
-      </c>
-    </row>
+        <v>1</v>
+      </c>
+      <c r="U51" s="19" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="52" customFormat="false" ht="19.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
@@ -7356,10 +7410,10 @@
   <dimension ref="A1:L61"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="10" sqref="E6 E9 E11:E12 E14 E18:E19 E23:E24 E26 E28 E36 E41:E42 A3"/>
+      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="26.74"/>
   </cols>

</xml_diff>